<commit_message>
Otimização do código e captura do nome do aluno do gabarito
</commit_message>
<xml_diff>
--- a/bancodedados/gabarito_teste4[Ciências da Natureza].xlsx
+++ b/bancodedados/gabarito_teste4[Ciências da Natureza].xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:C81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,12 +451,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve">   E</t>
+          <t xml:space="preserve">    E</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Peso</t>
+          <t>0.25</t>
         </is>
       </c>
     </row>
@@ -466,12 +466,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t xml:space="preserve">   C</t>
+          <t xml:space="preserve">    C</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Peso</t>
+          <t>0.25</t>
         </is>
       </c>
     </row>
@@ -481,12 +481,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t xml:space="preserve">   B</t>
+          <t xml:space="preserve">    B</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Peso</t>
+          <t>0.25</t>
         </is>
       </c>
     </row>
@@ -496,12 +496,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t xml:space="preserve">   B</t>
+          <t xml:space="preserve">    B</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Peso</t>
+          <t>0.25</t>
         </is>
       </c>
     </row>
@@ -511,12 +511,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t xml:space="preserve">   D</t>
+          <t xml:space="preserve">    D</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Peso</t>
+          <t>0.25</t>
         </is>
       </c>
     </row>
@@ -526,12 +526,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t xml:space="preserve">   B</t>
+          <t xml:space="preserve">    B</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Peso</t>
+          <t>0.25</t>
         </is>
       </c>
     </row>
@@ -541,12 +541,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t xml:space="preserve">   B</t>
+          <t xml:space="preserve">    B</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Peso</t>
+          <t>0.25</t>
         </is>
       </c>
     </row>
@@ -556,12 +556,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t xml:space="preserve">   D</t>
+          <t xml:space="preserve">    D</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Peso</t>
+          <t>0.25</t>
         </is>
       </c>
     </row>
@@ -571,12 +571,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t xml:space="preserve">   E</t>
+          <t xml:space="preserve">    E</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Peso</t>
+          <t>0.25</t>
         </is>
       </c>
     </row>
@@ -586,12 +586,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t xml:space="preserve">   E</t>
+          <t xml:space="preserve">    E</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Peso</t>
+          <t>0.25</t>
         </is>
       </c>
     </row>
@@ -601,12 +601,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t xml:space="preserve">   D</t>
+          <t xml:space="preserve">    D</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Peso</t>
+          <t>0.25</t>
         </is>
       </c>
     </row>
@@ -616,12 +616,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t xml:space="preserve">   C</t>
+          <t xml:space="preserve">    C</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Peso</t>
+          <t>0.25</t>
         </is>
       </c>
     </row>
@@ -631,12 +631,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t xml:space="preserve">   D</t>
+          <t xml:space="preserve">    D</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Peso</t>
+          <t>0.25</t>
         </is>
       </c>
     </row>
@@ -646,12 +646,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t xml:space="preserve">   B</t>
+          <t xml:space="preserve">    B</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Peso</t>
+          <t>0.25</t>
         </is>
       </c>
     </row>
@@ -661,12 +661,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t xml:space="preserve">   A</t>
+          <t xml:space="preserve">    A</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Peso</t>
+          <t>0.25</t>
         </is>
       </c>
     </row>
@@ -676,12 +676,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t xml:space="preserve">   A</t>
+          <t xml:space="preserve">    A</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Peso</t>
+          <t>0.25</t>
         </is>
       </c>
     </row>
@@ -691,12 +691,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t xml:space="preserve">   C</t>
+          <t xml:space="preserve">    C</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Peso</t>
+          <t>0.25</t>
         </is>
       </c>
     </row>
@@ -706,12 +706,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t xml:space="preserve">   B</t>
+          <t xml:space="preserve">    B</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Peso</t>
+          <t>0.25</t>
         </is>
       </c>
     </row>
@@ -721,12 +721,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t xml:space="preserve">   C</t>
+          <t xml:space="preserve">    C</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Peso</t>
+          <t>0.25</t>
         </is>
       </c>
     </row>
@@ -736,12 +736,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t xml:space="preserve">   C</t>
+          <t xml:space="preserve">    C</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Peso</t>
+          <t>0.25</t>
         </is>
       </c>
     </row>
@@ -751,12 +751,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t xml:space="preserve">   E</t>
+          <t xml:space="preserve">    E</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Peso</t>
+          <t>0.25</t>
         </is>
       </c>
     </row>
@@ -766,12 +766,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t xml:space="preserve">   C</t>
+          <t xml:space="preserve">    C</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Peso</t>
+          <t>0.25</t>
         </is>
       </c>
     </row>
@@ -781,12 +781,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t xml:space="preserve">   B</t>
+          <t xml:space="preserve">    B</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Peso</t>
+          <t>0.25</t>
         </is>
       </c>
     </row>
@@ -796,12 +796,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t xml:space="preserve">   B</t>
+          <t xml:space="preserve">    B</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Peso</t>
+          <t>0.25</t>
         </is>
       </c>
     </row>
@@ -811,12 +811,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t xml:space="preserve">   D</t>
+          <t xml:space="preserve">    D</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Peso</t>
+          <t>0.25</t>
         </is>
       </c>
     </row>
@@ -826,12 +826,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t xml:space="preserve">   B</t>
+          <t xml:space="preserve">    B</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Peso</t>
+          <t>0.25</t>
         </is>
       </c>
     </row>
@@ -841,12 +841,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t xml:space="preserve">   B</t>
+          <t xml:space="preserve">    B</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Peso</t>
+          <t>0.25</t>
         </is>
       </c>
     </row>
@@ -856,12 +856,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t xml:space="preserve">   D</t>
+          <t xml:space="preserve">    D</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Peso</t>
+          <t>0.25</t>
         </is>
       </c>
     </row>
@@ -871,12 +871,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t xml:space="preserve">   E</t>
+          <t xml:space="preserve">    E</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Peso</t>
+          <t>0.25</t>
         </is>
       </c>
     </row>
@@ -886,12 +886,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t xml:space="preserve">   E</t>
+          <t xml:space="preserve">    E</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Peso</t>
+          <t>0.25</t>
         </is>
       </c>
     </row>
@@ -901,12 +901,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t xml:space="preserve">   D</t>
+          <t xml:space="preserve">    D</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Peso</t>
+          <t>0.25</t>
         </is>
       </c>
     </row>
@@ -916,12 +916,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t xml:space="preserve">   C</t>
+          <t xml:space="preserve">    C</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Peso</t>
+          <t>0.25</t>
         </is>
       </c>
     </row>
@@ -931,12 +931,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t xml:space="preserve">   D</t>
+          <t xml:space="preserve">    D</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Peso</t>
+          <t>0.25</t>
         </is>
       </c>
     </row>
@@ -946,12 +946,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t xml:space="preserve">   B</t>
+          <t xml:space="preserve">    B</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Peso</t>
+          <t>0.25</t>
         </is>
       </c>
     </row>
@@ -961,12 +961,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t xml:space="preserve">   A</t>
+          <t xml:space="preserve">    A</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Peso</t>
+          <t>0.25</t>
         </is>
       </c>
     </row>
@@ -976,12 +976,12 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t xml:space="preserve">   A</t>
+          <t xml:space="preserve">    A</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Peso</t>
+          <t>0.25</t>
         </is>
       </c>
     </row>
@@ -991,12 +991,12 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t xml:space="preserve">   C</t>
+          <t xml:space="preserve">    C</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Peso</t>
+          <t>0.25</t>
         </is>
       </c>
     </row>
@@ -1006,12 +1006,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t xml:space="preserve">   B</t>
+          <t xml:space="preserve">    B</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Peso</t>
+          <t>0.25</t>
         </is>
       </c>
     </row>
@@ -1021,12 +1021,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t xml:space="preserve">   C</t>
+          <t xml:space="preserve">    C</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Peso</t>
+          <t>0.25</t>
         </is>
       </c>
     </row>
@@ -1036,12 +1036,612 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t xml:space="preserve">   C</t>
+          <t xml:space="preserve">    C</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Peso</t>
+          <t>0.25</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    E</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    C</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    B</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    B</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    D</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    B</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    B</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    D</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    E</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    E</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    D</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    C</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    D</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    B</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    A</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    A</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    C</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    B</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    C</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    C</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    E</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    C</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    B</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    B</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    D</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    B</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    B</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    D</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    E</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    E</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    D</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    C</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="n">
+        <v>72</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    D</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="n">
+        <v>73</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    B</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    A</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    A</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    C</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    B</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    C</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    C</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>0.25</t>
         </is>
       </c>
     </row>

</xml_diff>